<commit_message>
Added demo files for LR - RSS and TSS
Added demo files for LR - RSS and TSS
</commit_message>
<xml_diff>
--- a/1. Statistics and Machine Learning/8. Linear Regression/slr_excel_demonstration_1.xlsx
+++ b/1. Statistics and Machine Learning/8. Linear Regression/slr_excel_demonstration_1.xlsx
@@ -1,51 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karanpreet\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="5445"/>
+    <workbookView windowWidth="15990" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>SLOPE</t>
-  </si>
-  <si>
-    <t>INTERCEPT</t>
-  </si>
-  <si>
-    <t>RSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSS </t>
-  </si>
-  <si>
-    <t>R^2</t>
-  </si>
-  <si>
-    <t>Residual Squares</t>
-  </si>
-  <si>
-    <t>Sum of Squares</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
   <si>
     <t>Marketing Budget (X) (In lakhs)</t>
   </si>
@@ -55,17 +25,44 @@
   <si>
     <t>Predicted Sales (Y-pred)</t>
   </si>
+  <si>
+    <t>Residual Squares</t>
+  </si>
+  <si>
+    <t>Sum of Squares</t>
+  </si>
+  <si>
+    <t>SLOPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSS </t>
+  </si>
+  <si>
+    <t>INTERCEPT</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>RSS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -73,11 +70,162 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,12 +234,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -101,37 +435,279 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -139,26 +715,70 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -176,7 +796,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -202,6 +822,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -210,32 +831,12 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="marker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -262,6 +863,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -278,8 +882,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.13289370078740156"/>
-                  <c:y val="-0.16245370370370371"/>
+                  <c:x val="0.132893700787402"/>
+                  <c:y val="-0.162453703703704"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -288,7 +892,7 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                         <a:solidFill>
                           <a:schemeClr val="tx1">
                             <a:lumMod val="65000"/>
@@ -321,7 +925,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -333,7 +937,6 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -354,10 +957,10 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.69999999999999</c:v>
+                  <c:v>128.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>285.89999999999998</c:v>
+                  <c:v>285.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>200</c:v>
@@ -378,13 +981,13 @@
                   <c:v>297.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>256.39999999999998</c:v>
+                  <c:v>256.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>249.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>323.10000000000002</c:v>
+                  <c:v>323.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>223</c:v>
@@ -417,7 +1020,7 @@
                   <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>17.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12.5</c:v>
@@ -438,10 +1041,10 @@
                   <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.600000000000001</c:v>
+                  <c:v>16.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.100000000000001</c:v>
+                  <c:v>17.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>20.7</c:v>
@@ -459,11 +1062,6 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FAD7-4FB1-A536-41102CD29DF3}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -504,7 +1102,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -520,9 +1118,11 @@
                   <a:rPr lang="en-IN"/>
                   <a:t>Marketing Budget (In lakhs)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-IN"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -531,26 +1131,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -574,7 +1154,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -586,7 +1166,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="442885552"/>
@@ -621,7 +1200,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -637,9 +1216,11 @@
                   <a:rPr lang="en-IN"/>
                   <a:t>Sales (In crores)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-IN"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -648,26 +1229,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -691,7 +1252,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -703,7 +1264,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="442890472"/>
@@ -742,9 +1302,396 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="en-US"/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Sales(Y) (In crores)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>127.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>364.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>285.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>303.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>315.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>169.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>104.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>297.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>256.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>249.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>323.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="968105157"/>
+        <c:axId val="589456302"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="968105157"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="589456302"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="589456302"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="968105157"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US"/>
+      </a:pPr>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -795,6 +1742,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1311,8 +2298,524 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -1326,20 +2829,49 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="7810500" y="785495"/>
+        <a:ext cx="4572000" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3895725" y="1733550"/>
+        <a:ext cx="4572000" cy="2743200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1395,7 +2927,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1428,26 +2960,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1480,23 +2995,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1638,405 +3136,400 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.2857142857143" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="20.28515625" style="1"/>
+    <col min="1" max="1" width="29.4285714285714" style="4" customWidth="1"/>
+    <col min="2" max="3" width="23.4285714285714" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.8571428571429" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.4285714285714" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="20.2857142857143" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="1" s="3" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
         <v>127.4</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>10.5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>(B$20*A2+B$21)</f>
-        <v>10.079219999999999</v>
-      </c>
-      <c r="D2" s="3">
+        <v>10.07922</v>
+      </c>
+      <c r="D2" s="2">
         <f>(B2-C2)^2</f>
-        <v>0.17705580840000051</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+        <v>0.177055808400001</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
         <v>364.4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>21.4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <f t="shared" ref="C3:C18" si="0">(B$20*A3+B$21)</f>
-        <v>22.592819999999996</v>
-      </c>
-      <c r="D3" s="3">
+        <v>22.59282</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D18" si="1">(B3-C3)^2</f>
-        <v>1.4228195523999942</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+        <v>1.42281955239999</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
         <v>150</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>11.272500000000001</v>
-      </c>
-      <c r="D4" s="3">
+        <v>11.2725</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>1.6192562500000021</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>128.69999999999999</v>
-      </c>
-      <c r="B5" s="3">
+        <v>1.61925625</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>128.7</v>
+      </c>
+      <c r="B5" s="2">
         <v>9.6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>10.14786</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>0.30015057960000002</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>285.89999999999998</v>
-      </c>
-      <c r="B6" s="3">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="C6" s="3">
+        <v>0.3001505796</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>285.9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17.4</v>
+      </c>
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>18.44802</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>1.0983459204000021</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+        <v>1.0983459204</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
         <v>200</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>12.5</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>13.912500000000001</v>
-      </c>
-      <c r="D7" s="3">
+        <v>13.9125</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>1.995156250000004</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+        <v>1.99515625</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
         <v>303.3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>20</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>19.36674</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>0.40101822759999994</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+        <v>0.4010182276</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
         <v>315.7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>21</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>20.021459999999998</v>
-      </c>
-      <c r="D9" s="3">
+        <v>20.02146</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>0.95754053160000474</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+        <v>0.957540531600005</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
         <v>169.8</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>14.7</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>12.31794</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>5.6742098435999964</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+        <v>5.6742098436</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
         <v>104.9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>10.1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>8.8912200000000006</v>
-      </c>
-      <c r="D11" s="3">
+        <v>8.89122</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>1.4611490883999978</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+        <v>1.4611490884</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
         <v>297.7</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>21.5</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>19.071059999999999</v>
-      </c>
-      <c r="D12" s="3">
+        <v>19.07106</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>5.8997495236000042</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>256.39999999999998</v>
-      </c>
-      <c r="B13" s="3">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="C13" s="3">
+        <v>5.8997495236</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>256.4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>16.6</v>
+      </c>
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>16.890419999999999</v>
-      </c>
-      <c r="D13" s="3">
+        <v>16.89042</v>
+      </c>
+      <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>8.434377639999853E-2</v>
-      </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+        <v>0.0843437763999985</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
         <v>249.1</v>
       </c>
-      <c r="B14" s="3">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="2">
+        <v>17.1</v>
+      </c>
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>16.50498</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>0.35404880040000197</v>
-      </c>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>323.10000000000002</v>
-      </c>
-      <c r="B15" s="3">
+        <v>0.354048800400002</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>323.1</v>
+      </c>
+      <c r="B15" s="2">
         <v>20.7</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>20.412179999999999</v>
-      </c>
-      <c r="D15" s="3">
+        <v>20.41218</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>8.2840352399999984E-2</v>
-      </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+        <v>0.0828403524</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
         <v>223</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>15.5</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>15.126899999999999</v>
-      </c>
-      <c r="D16" s="3">
+        <v>15.1269</v>
+      </c>
+      <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>0.13920361000000064</v>
-      </c>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+        <v>0.139203610000001</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
         <v>235</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>13.5</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>15.7605</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>5.1098602500000014</v>
-      </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+        <v>5.10986025</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
         <v>200</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>12.5</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>13.912500000000001</v>
-      </c>
-      <c r="D18" s="3">
+        <v>13.9125</v>
+      </c>
+      <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>1.995156250000004</v>
-      </c>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.99515625</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B20" s="5">
-        <v>5.28E-2</v>
+        <v>0.0528</v>
       </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B21" s="5">
         <v>3.3525</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4">
         <f>SUM(D2:D18)</f>
-        <v>28.771904614800007</v>
+        <v>28.7719046148</v>
       </c>
       <c r="C22"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2044,8 +3537,183 @@
       <c r="E27" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="31.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="25.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="24.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="17.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2">
+        <v>127.4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <v>364.4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2">
+        <v>150</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2">
+        <v>128.7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2">
+        <v>285.9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>17.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2">
+        <v>200</v>
+      </c>
+      <c r="B7" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2">
+        <v>303.3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2">
+        <v>315.7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2">
+        <v>169.8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2">
+        <v>104.9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2">
+        <v>297.7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2">
+        <v>256.4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2">
+        <v>249.1</v>
+      </c>
+      <c r="B14" s="2">
+        <v>17.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="2">
+        <v>323.1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2">
+        <v>223</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2">
+        <v>235</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2">
+        <v>200</v>
+      </c>
+      <c r="B18" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>